<commit_message>
Actualizamos el archivo de excel
</commit_message>
<xml_diff>
--- a/estructurasDatosWordix..xlsx
+++ b/estructurasDatosWordix..xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27109"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0221ABD-4F1E-47A3-B570-224FD2812F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{943DCAB6-D92C-4FE6-A7DC-4243A53E91A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="59">
   <si>
     <t>$coleccionPalabras=</t>
   </si>
@@ -202,9 +202,6 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tipo: Multidimensional </t>
   </si>
   <si>
     <t>Tipos de datos: Almacena datos Asociativos que contienen cadenas de texto</t>
@@ -545,7 +542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -586,7 +583,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -914,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -936,128 +932,128 @@
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="29">
         <v>0</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="29">
         <v>1</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="29">
         <v>2</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="29">
         <v>3</v>
       </c>
-      <c r="F3" s="30">
+      <c r="F3" s="29">
         <v>4</v>
       </c>
-      <c r="G3" s="30">
+      <c r="G3" s="29">
         <v>5</v>
       </c>
-      <c r="H3" s="30">
+      <c r="H3" s="29">
         <v>6</v>
       </c>
-      <c r="I3" s="31">
+      <c r="I3" s="30">
         <v>7</v>
       </c>
-      <c r="J3" s="30">
+      <c r="J3" s="29">
         <v>8</v>
       </c>
-      <c r="K3" s="30">
+      <c r="K3" s="29">
         <v>9</v>
       </c>
-      <c r="L3" s="30">
+      <c r="L3" s="29">
         <v>10</v>
       </c>
-      <c r="M3" s="30">
+      <c r="M3" s="29">
         <v>11</v>
       </c>
-      <c r="N3" s="30">
+      <c r="N3" s="29">
         <v>12</v>
       </c>
-      <c r="O3" s="30">
+      <c r="O3" s="29">
         <v>13</v>
       </c>
-      <c r="P3" s="30">
+      <c r="P3" s="29">
         <v>14</v>
       </c>
-      <c r="Q3" s="30">
+      <c r="Q3" s="29">
         <v>15</v>
       </c>
-      <c r="R3" s="30">
+      <c r="R3" s="29">
         <v>16</v>
       </c>
-      <c r="S3" s="30">
+      <c r="S3" s="29">
         <v>17</v>
       </c>
-      <c r="T3" s="30">
+      <c r="T3" s="29">
         <v>18</v>
       </c>
-      <c r="U3" s="30">
+      <c r="U3" s="29">
         <v>19</v>
       </c>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
     </row>
     <row r="4" spans="1:24" ht="15.75">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="27" t="s">
+      <c r="J4" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="29" t="s">
+      <c r="K4" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="29" t="s">
+      <c r="L4" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="29" t="s">
+      <c r="M4" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="29" t="s">
+      <c r="N4" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="29" t="s">
+      <c r="O4" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="29" t="s">
+      <c r="P4" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="Q4" s="29" t="s">
+      <c r="Q4" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="R4" s="29" t="s">
+      <c r="R4" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="S4" s="29" t="s">
+      <c r="S4" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="T4" s="29" t="s">
+      <c r="T4" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="U4" s="29" t="s">
+      <c r="U4" s="28" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1105,73 +1101,73 @@
       <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="32">
+      <c r="B13" s="31">
         <v>0</v>
       </c>
-      <c r="C13" s="32">
+      <c r="C13" s="31">
         <v>1</v>
       </c>
-      <c r="D13" s="32">
+      <c r="D13" s="31">
         <v>2</v>
       </c>
-      <c r="E13" s="32">
+      <c r="E13" s="31">
         <v>3</v>
       </c>
-      <c r="F13" s="32">
+      <c r="F13" s="31">
         <v>4</v>
       </c>
-      <c r="G13" s="32">
+      <c r="G13" s="31">
         <v>5</v>
       </c>
-      <c r="H13" s="32">
+      <c r="H13" s="31">
         <v>6</v>
       </c>
-      <c r="I13" s="32">
+      <c r="I13" s="31">
         <v>7</v>
       </c>
-      <c r="J13" s="32">
+      <c r="J13" s="31">
         <v>8</v>
       </c>
-      <c r="K13" s="32">
+      <c r="K13" s="31">
         <v>9</v>
       </c>
-      <c r="L13" s="32">
+      <c r="L13" s="31">
         <v>10</v>
       </c>
-      <c r="M13" s="33">
+      <c r="M13" s="32">
         <v>11</v>
       </c>
-      <c r="N13" s="34">
+      <c r="N13" s="33">
         <v>12</v>
       </c>
-      <c r="O13" s="34">
+      <c r="O13" s="33">
         <v>13</v>
       </c>
-      <c r="P13" s="34">
+      <c r="P13" s="33">
         <v>14</v>
       </c>
-      <c r="Q13" s="34">
+      <c r="Q13" s="33">
         <v>15</v>
       </c>
-      <c r="R13" s="34">
+      <c r="R13" s="33">
         <v>16</v>
       </c>
-      <c r="S13" s="34">
+      <c r="S13" s="33">
         <v>17</v>
       </c>
-      <c r="T13" s="34">
+      <c r="T13" s="33">
         <v>18</v>
       </c>
-      <c r="U13" s="34">
+      <c r="U13" s="33">
         <v>19</v>
       </c>
-      <c r="V13" s="34">
+      <c r="V13" s="33">
         <v>20</v>
       </c>
-      <c r="W13" s="34">
+      <c r="W13" s="33">
         <v>21</v>
       </c>
-      <c r="X13" s="34">
+      <c r="X13" s="33">
         <v>22</v>
       </c>
     </row>
@@ -1615,7 +1611,7 @@
       <c r="B35" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="35" t="s">
+      <c r="C35" s="34" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1723,7 +1719,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="2:7" ht="15" customHeight="1">
+    <row r="49" spans="2:6" ht="15" customHeight="1">
       <c r="B49" s="4" t="s">
         <v>5</v>
       </c>
@@ -1731,7 +1727,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="50" spans="2:7" ht="15" customHeight="1">
+    <row r="50" spans="2:6" ht="15" customHeight="1">
       <c r="B50" s="4" t="s">
         <v>18</v>
       </c>
@@ -1739,7 +1735,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="2:7" ht="15" customHeight="1">
+    <row r="51" spans="2:6" ht="15" customHeight="1">
       <c r="B51" s="4" t="s">
         <v>3</v>
       </c>
@@ -1747,7 +1743,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="2:7" ht="15" customHeight="1">
+    <row r="52" spans="2:6" ht="15" customHeight="1">
       <c r="B52" s="4" t="s">
         <v>19</v>
       </c>
@@ -1755,7 +1751,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="2:7" ht="15" customHeight="1">
+    <row r="53" spans="2:6" ht="15" customHeight="1">
       <c r="B53" s="4" t="s">
         <v>10</v>
       </c>
@@ -1763,7 +1759,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="2:7" ht="15" customHeight="1">
+    <row r="54" spans="2:6" ht="15" customHeight="1">
       <c r="B54" s="4" t="s">
         <v>8</v>
       </c>
@@ -1771,7 +1767,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="2:7" ht="15" customHeight="1">
+    <row r="55" spans="2:6" ht="15" customHeight="1">
       <c r="B55" s="4" t="s">
         <v>13</v>
       </c>
@@ -1779,7 +1775,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="2:7" ht="15" customHeight="1">
+    <row r="56" spans="2:6" ht="15" customHeight="1">
       <c r="B56" s="4" t="s">
         <v>14</v>
       </c>
@@ -1787,7 +1783,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="57" spans="2:7" ht="15" customHeight="1">
+    <row r="57" spans="2:6" ht="15" customHeight="1">
       <c r="B57" s="4" t="s">
         <v>26</v>
       </c>
@@ -1795,7 +1791,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="58" spans="2:7" ht="15" customHeight="1">
+    <row r="58" spans="2:6" ht="15" customHeight="1">
       <c r="B58" s="4" t="s">
         <v>17</v>
       </c>
@@ -1803,12 +1799,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="2:7" ht="15" customHeight="1">
+    <row r="59" spans="2:6" ht="15" customHeight="1">
       <c r="C59" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="2:7" ht="15" customHeight="1">
+    <row r="60" spans="2:6" ht="15" customHeight="1">
       <c r="B60" s="20" t="s">
         <v>20</v>
       </c>
@@ -1817,35 +1813,34 @@
       <c r="E60" s="18"/>
       <c r="F60" s="19"/>
     </row>
-    <row r="61" spans="2:7" ht="15" customHeight="1">
+    <row r="61" spans="2:6" ht="15" customHeight="1">
       <c r="B61" s="6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C61" s="18"/>
       <c r="D61" s="18"/>
       <c r="E61" s="18"/>
       <c r="F61" s="19"/>
     </row>
-    <row r="62" spans="2:7" ht="15" customHeight="1">
+    <row r="62" spans="2:6" ht="15" customHeight="1">
       <c r="B62" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C62" s="18"/>
       <c r="D62" s="18"/>
       <c r="E62" s="18"/>
       <c r="F62" s="19"/>
     </row>
-    <row r="63" spans="2:7" ht="15" customHeight="1">
+    <row r="63" spans="2:6" ht="15" customHeight="1">
       <c r="B63" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
-      <c r="G63" s="26"/>
-    </row>
-    <row r="64" spans="2:7" ht="15" customHeight="1">
+    </row>
+    <row r="64" spans="2:6" ht="15" customHeight="1">
       <c r="C64" t="s">
         <v>56</v>
       </c>

</xml_diff>